<commit_message>
Avances hasta día del comité
</commit_message>
<xml_diff>
--- a/atm_data/sk_uncertainties_data.xlsx
+++ b/atm_data/sk_uncertainties_data.xlsx
@@ -886,8 +886,8 @@
   </sheetPr>
   <dimension ref="B1:J196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F181" activeCellId="0" sqref="F181"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F192" activeCellId="0" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>